<commit_message>
Updated spreadsheets, removed unnecessary print
</commit_message>
<xml_diff>
--- a/bitcoin_hash/finalsummary.xlsx
+++ b/bitcoin_hash/finalsummary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alanmohamad/Desktop/ECE 111/ece_111_final_project/bitcoin_hash/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\me\Documents\ece_111_final_project\bitcoin_hash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86653159-FA58-7640-82FC-9F947E09668E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1301563C-D0C6-477B-96FF-9D0EA0AFB225}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30020" windowHeight="16720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Last Name</t>
   </si>
@@ -110,9 +110,6 @@
     <t>amohamad@ucsd.edu</t>
   </si>
   <si>
-    <t>Balanced</t>
-  </si>
-  <si>
     <t>Young</t>
   </si>
   <si>
@@ -120,6 +117,15 @@
   </si>
   <si>
     <t>aryoung@ucsd.edu</t>
+  </si>
+  <si>
+    <t>A17210559</t>
+  </si>
+  <si>
+    <t>Area (Aggressive)</t>
+  </si>
+  <si>
+    <t>Note: we also changed additional compiler settings (fitter effort, etc). Have included QPF files for reference.</t>
   </si>
 </sst>
 </file>
@@ -1119,34 +1125,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U4"/>
+  <dimension ref="A1:U6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="216" zoomScaleNormal="216" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="17.83203125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="9.83203125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.83203125" style="2" customWidth="1"/>
-    <col min="9" max="11" width="9.83203125" style="2" customWidth="1"/>
-    <col min="12" max="12" width="10.83203125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="13.83203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.85546875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="9.85546875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" style="2" customWidth="1"/>
+    <col min="9" max="11" width="9.85546875" style="2" customWidth="1"/>
+    <col min="12" max="12" width="10.85546875" style="3" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" style="3" customWidth="1"/>
     <col min="14" max="14" width="25" style="3" customWidth="1"/>
-    <col min="15" max="15" width="9.83203125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="2" customWidth="1"/>
-    <col min="17" max="19" width="9.83203125" style="2" customWidth="1"/>
-    <col min="20" max="20" width="10.83203125" style="3" customWidth="1"/>
-    <col min="21" max="21" width="13.83203125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" style="2" customWidth="1"/>
+    <col min="16" max="16" width="10.85546875" style="2" customWidth="1"/>
+    <col min="17" max="19" width="9.85546875" style="2" customWidth="1"/>
+    <col min="20" max="20" width="10.85546875" style="3" customWidth="1"/>
+    <col min="21" max="21" width="13.85546875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="14"/>
       <c r="B1" s="15"/>
       <c r="C1" s="15"/>
@@ -1171,7 +1177,7 @@
       <c r="T1" s="15"/>
       <c r="U1" s="16"/>
     </row>
-    <row r="2" spans="1:21" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:21" s="11" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
@@ -1220,7 +1226,7 @@
       <c r="T2" s="10"/>
       <c r="U2" s="10"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>14</v>
       </c>
@@ -1237,31 +1243,31 @@
         <v>18</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G3" s="4">
-        <v>14831</v>
+        <v>14717</v>
       </c>
       <c r="H3" s="4">
         <v>21683</v>
       </c>
       <c r="I3" s="5">
         <f>G3+H3</f>
-        <v>36514</v>
+        <v>36400</v>
       </c>
       <c r="J3" s="6">
-        <v>107.83</v>
+        <v>114.44</v>
       </c>
       <c r="K3" s="4">
         <v>241</v>
       </c>
       <c r="L3" s="7">
         <f>K3/J3</f>
-        <v>2.23499953630715</v>
+        <v>2.1059070255155539</v>
       </c>
       <c r="M3" s="7">
         <f t="shared" ref="M3" si="0">I3*L3/1000</f>
-        <v>81.608773068719287</v>
+        <v>76.655015728766159</v>
       </c>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
@@ -1272,46 +1278,48 @@
       <c r="T3" s="7"/>
       <c r="U3" s="7"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="D4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G4" s="4">
-        <v>14831</v>
+        <v>14717</v>
       </c>
       <c r="H4" s="4">
         <v>21683</v>
       </c>
       <c r="I4" s="5">
         <f>G4+H4</f>
-        <v>36514</v>
+        <v>36400</v>
       </c>
       <c r="J4" s="6">
-        <v>107.83</v>
+        <v>114.44</v>
       </c>
       <c r="K4" s="4">
         <v>241</v>
       </c>
       <c r="L4" s="7">
         <f>K4/J4</f>
-        <v>2.23499953630715</v>
+        <v>2.1059070255155539</v>
       </c>
       <c r="M4" s="7">
         <f t="shared" ref="M4" si="1">I4*L4/1000</f>
-        <v>81.608773068719287</v>
+        <v>76.655015728766159</v>
       </c>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -1321,6 +1329,11 @@
       <c r="S4" s="4"/>
       <c r="T4" s="7"/>
       <c r="U4" s="7"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>